<commit_message>
Added Carla to CSV Onboard reading file
</commit_message>
<xml_diff>
--- a/0-Onboard/Onboard_Reading.xlsx
+++ b/0-Onboard/Onboard_Reading.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexc\Pictures\Geotab\ComputerVision_Mapping\0-Onboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{316CAE6A-AD5B-488F-90AD-AD5D11B391FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BFC9D0-3E7E-4148-A20E-F0D493AFAD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="20460" windowHeight="10920" xr2:uid="{05B7A4B9-903E-43E7-B9B2-B23D6730C73F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{05B7A4B9-903E-43E7-B9B2-B23D6730C73F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Link</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>Optional</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLQVvvaa0QuDeI12McNQdnTlWz9XlCa0uo</t>
+  </si>
+  <si>
+    <t>CARLA (First 2 videos)</t>
+  </si>
+  <si>
+    <t>1:00 Hrs</t>
   </si>
 </sst>
 </file>
@@ -510,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEFB5AC-8A62-48C6-9E49-01433BD2DB60}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,80 +593,97 @@
         <v>30</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>14</v>
       </c>
     </row>
@@ -666,8 +692,9 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{402A9D6C-CEEA-496D-87DF-EAE8BF07ECEA}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{C70EF42B-5753-4B03-A5DE-6F2D67638294}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{E376158D-3507-4C01-A9EA-EF6A7D626E26}"/>
+    <hyperlink ref="B6" r:id="rId4" tooltip="https://www.youtube.com/playlist?list=plqvvvaa0qudei12mcnqdntlwz9xlca0uo" xr:uid="{5FB6D2E2-CD0E-46FA-8C51-3699D2580FC3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created onboarding word document
</commit_message>
<xml_diff>
--- a/0-Onboard/Onboard_Reading.xlsx
+++ b/0-Onboard/Onboard_Reading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexc\Pictures\Geotab\ComputerVision_Mapping\0-Onboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BFC9D0-3E7E-4148-A20E-F0D493AFAD62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D13E20-1C4A-47C7-AD5D-77F458A9ED82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{05B7A4B9-903E-43E7-B9B2-B23D6730C73F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="38">
   <si>
     <t>Link</t>
   </si>
@@ -72,12 +72,6 @@
     <t>Read Length</t>
   </si>
   <si>
-    <t>https://cloud.google.com/vision</t>
-  </si>
-  <si>
-    <t>Google Cloud Vision</t>
-  </si>
-  <si>
     <t>10 Min</t>
   </si>
   <si>
@@ -136,6 +130,24 @@
   </si>
   <si>
     <t>1:00 Hrs</t>
+  </si>
+  <si>
+    <t>Angular</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/learning/paths/advance-your-angular-skills?accountId=2272289&amp;u=2272289&amp;success=true&amp;authUUID=QqzIjcSKTcmt%2FdC30tftyw%3D%3D</t>
+  </si>
+  <si>
+    <t>8:00 Hrs</t>
+  </si>
+  <si>
+    <t>Yolo V5 Tutorial</t>
+  </si>
+  <si>
+    <t>https://colab.research.google.com/github/ultralytics/yolov5/blob/master/tutorial.ipynb</t>
+  </si>
+  <si>
+    <t>15 Min</t>
   </si>
 </sst>
 </file>
@@ -519,16 +531,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CEFB5AC-8A62-48C6-9E49-01433BD2DB60}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="98.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="106.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -567,124 +579,138 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" t="s">
         <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
         <v>21</v>
       </c>
-      <c r="C12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
+      <c r="C19" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -693,8 +719,9 @@
     <hyperlink ref="B3" r:id="rId2" xr:uid="{C70EF42B-5753-4B03-A5DE-6F2D67638294}"/>
     <hyperlink ref="B5" r:id="rId3" xr:uid="{E376158D-3507-4C01-A9EA-EF6A7D626E26}"/>
     <hyperlink ref="B6" r:id="rId4" tooltip="https://www.youtube.com/playlist?list=plqvvvaa0qudei12mcnqdntlwz9xlca0uo" xr:uid="{5FB6D2E2-CD0E-46FA-8C51-3699D2580FC3}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{D7A89B0F-F7BD-423F-A79B-64B5917ADB27}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>